<commit_message>
new DNN result files
</commit_message>
<xml_diff>
--- a/beijing/small_domain/descreptive-analysis.xlsx
+++ b/beijing/small_domain/descreptive-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\data\beijing\small_domain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35229AC7-3021-44F5-A65E-D8D6437A2893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDE82E5-E4BE-48FE-AC3E-E93837B544A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2753" yWindow="2168" windowWidth="14047" windowHeight="11249" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_abs_all" sheetId="1" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
@@ -49106,8 +49106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F366"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -49192,6 +49192,7 @@
       <c r="D4" s="1">
         <v>-31.0899999999999</v>
       </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
@@ -54264,6 +54265,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>